<commit_message>
Added skeletons of tests, failing tests for testTargets, changed players to ArrayList, small fix to person.txt
</commit_message>
<xml_diff>
--- a/BoardLayout_highlight_starts.xlsx
+++ b/BoardLayout_highlight_starts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameITCM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\csci306\forkITCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -187,31 +187,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF663300"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,12 +438,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,7 +732,7 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +753,7 @@
       <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="47" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="36" t="s">
@@ -789,7 +789,7 @@
       <c r="P1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -1345,7 +1345,7 @@
       <c r="T9" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="U9" s="48" t="s">
+      <c r="U9" s="44" t="s">
         <v>1</v>
       </c>
       <c r="V9">
@@ -1421,7 +1421,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -2184,7 +2184,7 @@
       <c r="E22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="46" t="s">
+      <c r="F22" s="45" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="25" t="s">
@@ -2214,7 +2214,7 @@
       <c r="O22" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="P22" s="44" t="s">
+      <c r="P22" s="46" t="s">
         <v>1</v>
       </c>
       <c r="Q22" s="34" t="s">

</xml_diff>

<commit_message>
changed color of board
</commit_message>
<xml_diff>
--- a/BoardLayout_highlight_starts.xlsx
+++ b/BoardLayout_highlight_starts.xlsx
@@ -136,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,18 +164,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -429,21 +417,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,7 +715,7 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,10 +736,10 @@
       <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -789,7 +772,7 @@
       <c r="P1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -883,7 +866,7 @@
       <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="22" t="s">
@@ -1025,10 +1008,10 @@
       <c r="D5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="37" t="s">
+      <c r="E5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="30" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -1052,7 +1035,7 @@
       <c r="M5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="22" t="s">
         <v>1</v>
       </c>
       <c r="O5" s="7" t="s">
@@ -1081,7 +1064,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
@@ -1226,7 +1209,7 @@
       <c r="C8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="22" t="s">
@@ -1262,7 +1245,7 @@
       <c r="O8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="22" t="s">
         <v>1</v>
       </c>
       <c r="Q8" s="22" t="s">
@@ -1342,10 +1325,10 @@
       <c r="S9" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="T9" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="U9" s="44" t="s">
+      <c r="T9" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" s="38" t="s">
         <v>1</v>
       </c>
       <c r="V9">
@@ -1421,7 +1404,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -1472,7 +1455,7 @@
       <c r="Q11" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="R11" s="40" t="s">
+      <c r="R11" s="34" t="s">
         <v>11</v>
       </c>
       <c r="S11" s="2" t="s">
@@ -1492,7 +1475,7 @@
       <c r="A12" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="22" t="s">
@@ -1543,7 +1526,7 @@
       <c r="R12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S12" s="42" t="s">
+      <c r="S12" s="36" t="s">
         <v>8</v>
       </c>
       <c r="T12" s="5" t="s">
@@ -1750,7 +1733,7 @@
       <c r="S15" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="T15" s="41" t="s">
+      <c r="T15" s="35" t="s">
         <v>25</v>
       </c>
       <c r="U15" s="9" t="s">
@@ -1838,7 +1821,7 @@
       <c r="C17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="43" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="22" t="s">
@@ -1868,7 +1851,7 @@
       <c r="M17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N17" s="42" t="s">
+      <c r="N17" s="36" t="s">
         <v>13</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -1942,7 +1925,7 @@
       <c r="O18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P18" s="35" t="s">
+      <c r="P18" s="22" t="s">
         <v>1</v>
       </c>
       <c r="Q18" s="22" t="s">
@@ -2087,7 +2070,7 @@
       <c r="R20" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="S20" s="42" t="s">
+      <c r="S20" s="36" t="s">
         <v>12</v>
       </c>
       <c r="T20" s="5" t="s">
@@ -2184,7 +2167,7 @@
       <c r="E22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="45" t="s">
+      <c r="F22" s="39" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="25" t="s">
@@ -2214,10 +2197,10 @@
       <c r="O22" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="P22" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="34" t="s">
+      <c r="P22" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="25" t="s">
         <v>1</v>
       </c>
       <c r="R22" s="7" t="s">

</xml_diff>

<commit_message>
Added failing tests for creating suggestions
</commit_message>
<xml_diff>
--- a/BoardLayout_highlight_starts.xlsx
+++ b/BoardLayout_highlight_starts.xlsx
@@ -120,7 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +131,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -382,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -427,6 +433,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,7 +722,7 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1533,7 @@
       <c r="R12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S12" s="36" t="s">
+      <c r="S12" s="44" t="s">
         <v>8</v>
       </c>
       <c r="T12" s="5" t="s">

</xml_diff>